<commit_message>
enlarge amount of total money
</commit_message>
<xml_diff>
--- a/backtest/bt_report/bs_voq_rs_m_style_28/single_run/summary.xlsx
+++ b/backtest/bt_report/bs_voq_rs_m_style_28/single_run/summary.xlsx
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="B8" s="7" t="n">
-        <v>39238106.520998</v>
+        <v>39168469.1083668</v>
       </c>
       <c r="C8" s="13" t="n"/>
       <c r="D8" s="13" t="n"/>
@@ -726,7 +726,7 @@
         </is>
       </c>
       <c r="B9" s="7" t="n">
-        <v>2453.259998003865</v>
+        <v>919.7378668054007</v>
       </c>
       <c r="C9" s="13" t="n"/>
       <c r="D9" s="13" t="n"/>
@@ -740,7 +740,7 @@
         </is>
       </c>
       <c r="B10" s="7" t="n">
-        <v>2.9238106520998</v>
+        <v>2.91684691083668</v>
       </c>
       <c r="C10" s="13" t="n"/>
       <c r="D10" s="13" t="n"/>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="B11" s="7" t="n">
-        <v>0.187974759056674</v>
+        <v>0.1877089012557587</v>
       </c>
       <c r="C11" s="13" t="n"/>
       <c r="D11" s="13" t="n"/>
@@ -768,7 +768,7 @@
         </is>
       </c>
       <c r="B12" s="7" t="n">
-        <v>3.9238106520998</v>
+        <v>3.91684691083668</v>
       </c>
       <c r="C12" s="13" t="n"/>
       <c r="D12" s="13" t="n"/>
@@ -796,7 +796,7 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>90.34805307159105</v>
+        <v>89.46681653096785</v>
       </c>
       <c r="C14" s="13" t="n"/>
       <c r="D14" s="13" t="n"/>
@@ -810,7 +810,7 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>0.1141132788720286</v>
+        <v>0.2187656891957522</v>
       </c>
     </row>
     <row r="16" ht="20" customHeight="1">
@@ -820,7 +820,7 @@
         </is>
       </c>
       <c r="B16" s="5" t="n">
-        <v>0.1412871132642348</v>
+        <v>0.141625944128847</v>
       </c>
       <c r="C16" s="13" t="n"/>
       <c r="D16" s="13" t="n"/>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="B17" s="5" t="n">
-        <v>0.9856290999719012</v>
+        <v>0.9820351689328671</v>
       </c>
       <c r="C17" s="13" t="n"/>
       <c r="D17" s="13" t="n"/>
@@ -848,7 +848,7 @@
         </is>
       </c>
       <c r="B18" s="5" t="n">
-        <v>0.09694069082244466</v>
+        <v>0.09724832525025326</v>
       </c>
       <c r="C18" s="13" t="n"/>
       <c r="D18" s="13" t="n"/>
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="B19" s="5" t="n">
-        <v>1.436514317185097</v>
+        <v>1.430170212288431</v>
       </c>
       <c r="C19" s="13" t="n"/>
       <c r="D19" s="13" t="n"/>
@@ -876,7 +876,7 @@
         </is>
       </c>
       <c r="B20" s="5" t="n">
-        <v>0.1484820596725185</v>
+        <v>0.1495147817574969</v>
       </c>
       <c r="C20" s="13" t="n"/>
       <c r="D20" s="13" t="n"/>
@@ -890,7 +890,7 @@
         </is>
       </c>
       <c r="B21" s="5" t="n">
-        <v>0.01405042335016219</v>
+        <v>0.01408808139083162</v>
       </c>
       <c r="C21" s="13" t="n"/>
       <c r="D21" s="13" t="n"/>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="B22" s="7" t="n">
-        <v>0.08862449372705219</v>
+        <v>0.08701204795218487</v>
       </c>
       <c r="C22" s="13" t="n"/>
       <c r="D22" s="13" t="n"/>
@@ -918,7 +918,7 @@
         </is>
       </c>
       <c r="B23" s="7" t="n">
-        <v>0.0107567278775218</v>
+        <v>0.01056796982848396</v>
       </c>
       <c r="C23" s="13" t="n"/>
       <c r="D23" s="13" t="n"/>
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="B24" s="7" t="n">
-        <v>0.130728522652875</v>
+        <v>0.1304439779736092</v>
       </c>
       <c r="C24" s="13" t="n"/>
       <c r="D24" s="13" t="n"/>
@@ -946,7 +946,7 @@
         </is>
       </c>
       <c r="B25" s="7" t="n">
-        <v>0.2688461232073023</v>
+        <v>0.2692243933206073</v>
       </c>
       <c r="C25" s="13" t="n"/>
       <c r="D25" s="13" t="n"/>
@@ -960,7 +960,7 @@
         </is>
       </c>
       <c r="B26" s="7" t="n">
-        <v>1.438580331352379</v>
+        <v>1.431696530792897</v>
       </c>
       <c r="C26" s="13" t="n"/>
       <c r="D26" s="13" t="n"/>
@@ -974,7 +974,7 @@
         </is>
       </c>
       <c r="B27" s="7" t="n">
-        <v>0.1691316013947884</v>
+        <v>0.1684214540400182</v>
       </c>
       <c r="C27" s="13" t="n"/>
       <c r="D27" s="13" t="n"/>
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="B28" s="7" t="n">
-        <v>0.5230969731855649</v>
+        <v>0.5231245654590744</v>
       </c>
       <c r="C28" s="13" t="n"/>
       <c r="D28" s="13" t="n"/>
@@ -1002,7 +1002,7 @@
         </is>
       </c>
       <c r="B29" s="7" t="n">
-        <v>0.2562312254163807</v>
+        <v>0.2562723698808536</v>
       </c>
       <c r="C29" s="13" t="n"/>
       <c r="D29" s="13" t="n"/>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B30" s="5" t="n">
-        <v>0.1252175775227669</v>
+        <v>0.1249451171768549</v>
       </c>
       <c r="C30" s="13" t="n"/>
       <c r="D30" s="13" t="n"/>
@@ -1030,7 +1030,7 @@
         </is>
       </c>
       <c r="B31" s="5" t="n">
-        <v>0.3024302585956767</v>
+        <v>0.302714639089421</v>
       </c>
       <c r="C31" s="13" t="n"/>
       <c r="D31" s="13" t="n"/>
@@ -1044,7 +1044,7 @@
         </is>
       </c>
       <c r="B32" s="5" t="n">
-        <v>0.9695718576465068</v>
+        <v>0.9664077004093462</v>
       </c>
       <c r="C32" s="13" t="n"/>
       <c r="D32" s="13" t="n"/>
@@ -1058,7 +1058,7 @@
         </is>
       </c>
       <c r="B33" s="5" t="n">
-        <v>1.459233437545993</v>
+        <v>1.454609450497398</v>
       </c>
     </row>
     <row r="34" ht="20" customHeight="1">
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="B34" s="5" t="n">
-        <v>1.46355769556389</v>
+        <v>1.457065520755955</v>
       </c>
     </row>
     <row r="35" ht="20" customHeight="1">
@@ -1078,7 +1078,7 @@
         </is>
       </c>
       <c r="B35" s="5" t="n">
-        <v>0.03242920619457007</v>
+        <v>0.03243637542664235</v>
       </c>
     </row>
     <row r="36" ht="20" customHeight="1">
@@ -1088,7 +1088,7 @@
         </is>
       </c>
       <c r="B36" s="16" t="n">
-        <v>0.1263998213314886</v>
+        <v>0.1274426875198475</v>
       </c>
     </row>
   </sheetData>
@@ -1157,16 +1157,16 @@
         <v>2014</v>
       </c>
       <c r="B2" s="13" t="n">
-        <v>0.3306780000000009</v>
+        <v>0.3313060000000018</v>
       </c>
       <c r="C2" s="13" t="n">
-        <v>0.1989033221052341</v>
+        <v>0.1994736432261886</v>
       </c>
       <c r="D2" s="13" t="n">
-        <v>3.239185391286652</v>
+        <v>3.235016309364732</v>
       </c>
       <c r="E2" s="13" t="n">
-        <v>4.274517950738013</v>
+        <v>4.269053056892319</v>
       </c>
       <c r="F2" s="13" t="n">
         <v>0.4473684210526316</v>
@@ -1177,16 +1177,16 @@
         <v>2015</v>
       </c>
       <c r="B3" s="13" t="n">
-        <v>0.7608121574114834</v>
+        <v>0.7604788080276035</v>
       </c>
       <c r="C3" s="13" t="n">
-        <v>-0.1935830927245927</v>
+        <v>-0.1936258076237396</v>
       </c>
       <c r="D3" s="13" t="n">
-        <v>2.34768906678677</v>
+        <v>2.338215455423227</v>
       </c>
       <c r="E3" s="13" t="n">
-        <v>2.456401924229428</v>
+        <v>2.438416194695802</v>
       </c>
       <c r="F3" s="13" t="n">
         <v>0.3461538461538461</v>
@@ -1197,16 +1197,16 @@
         <v>2016</v>
       </c>
       <c r="B4" s="13" t="n">
-        <v>-0.03678244903916856</v>
+        <v>-0.03790614642604755</v>
       </c>
       <c r="C4" s="13" t="n">
-        <v>0.2098900147957224</v>
+        <v>0.2085366623745854</v>
       </c>
       <c r="D4" s="13" t="n">
-        <v>-0.3029734605474155</v>
+        <v>-0.3134596616348824</v>
       </c>
       <c r="E4" s="13" t="n">
-        <v>0.01575817183538588</v>
+        <v>0.00510454002444844</v>
       </c>
       <c r="F4" s="13" t="n">
         <v>0.5</v>
@@ -1217,16 +1217,16 @@
         <v>2017</v>
       </c>
       <c r="B5" s="13" t="n">
-        <v>0.01077367527881256</v>
+        <v>0.01071314216987606</v>
       </c>
       <c r="C5" s="13" t="n">
-        <v>0.1025483142535694</v>
+        <v>0.1024794944331828</v>
       </c>
       <c r="D5" s="13" t="n">
-        <v>0.7331575191261513</v>
+        <v>0.7280028750631081</v>
       </c>
       <c r="E5" s="13" t="n">
-        <v>0.8887398168216636</v>
+        <v>0.8822013553661702</v>
       </c>
       <c r="F5" s="13" t="n">
         <v>0.5686274509803921</v>
@@ -1237,16 +1237,16 @@
         <v>2018</v>
       </c>
       <c r="B6" s="13" t="n">
-        <v>-0.04504198438982805</v>
+        <v>-0.04541627194827867</v>
       </c>
       <c r="C6" s="13" t="n">
-        <v>0.2620289966455215</v>
+        <v>0.2615620509137705</v>
       </c>
       <c r="D6" s="13" t="n">
-        <v>-0.394430785352302</v>
+        <v>-0.3981301425712103</v>
       </c>
       <c r="E6" s="13" t="n">
-        <v>0.2224536763300912</v>
+        <v>0.2190615047206603</v>
       </c>
       <c r="F6" s="13" t="n">
         <v>0.6078431372549019</v>
@@ -1257,16 +1257,16 @@
         <v>2019</v>
       </c>
       <c r="B7" s="13" t="n">
-        <v>0.2049750855537522</v>
+        <v>0.2048649878536174</v>
       </c>
       <c r="C7" s="13" t="n">
-        <v>-0.1979426892623817</v>
+        <v>-0.197981990523357</v>
       </c>
       <c r="D7" s="13" t="n">
-        <v>1.684483585157296</v>
+        <v>1.681319350626908</v>
       </c>
       <c r="E7" s="13" t="n">
-        <v>0.740386504597042</v>
+        <v>0.7344585164268693</v>
       </c>
       <c r="F7" s="13" t="n">
         <v>0.4423076923076923</v>
@@ -1277,16 +1277,16 @@
         <v>2020</v>
       </c>
       <c r="B8" s="13" t="n">
-        <v>0.298917250543241</v>
+        <v>0.2987351778052976</v>
       </c>
       <c r="C8" s="13" t="n">
-        <v>-0.2547192050654234</v>
+        <v>-0.2548117160557012</v>
       </c>
       <c r="D8" s="13" t="n">
-        <v>1.776441043050368</v>
+        <v>1.774902306674777</v>
       </c>
       <c r="E8" s="13" t="n">
-        <v>0.3010288730462792</v>
+        <v>0.2976202126007806</v>
       </c>
       <c r="F8" s="13" t="n">
         <v>0.4230769230769231</v>
@@ -1297,16 +1297,16 @@
         <v>2021</v>
       </c>
       <c r="B9" s="13" t="n">
-        <v>0.01676894050598335</v>
+        <v>0.01648800015509863</v>
       </c>
       <c r="C9" s="13" t="n">
-        <v>-0.1354903792359427</v>
+        <v>-0.135712148745459</v>
       </c>
       <c r="D9" s="13" t="n">
-        <v>0.199177757579037</v>
+        <v>0.1968861690784366</v>
       </c>
       <c r="E9" s="13" t="n">
-        <v>-0.3051327379875225</v>
+        <v>-0.3089724637462825</v>
       </c>
       <c r="F9" s="13" t="n">
         <v>0.4038461538461539</v>
@@ -1317,16 +1317,16 @@
         <v>2022</v>
       </c>
       <c r="B10" s="13" t="n">
-        <v>0.1318207817958449</v>
+        <v>0.1318979986267564</v>
       </c>
       <c r="C10" s="13" t="n">
-        <v>0.294274232713105</v>
+        <v>0.2943733801949364</v>
       </c>
       <c r="D10" s="13" t="n">
-        <v>2.951507110223165</v>
+        <v>2.949438514723716</v>
       </c>
       <c r="E10" s="13" t="n">
-        <v>4.115502945106555</v>
+        <v>4.113346547261292</v>
       </c>
       <c r="F10" s="13" t="n">
         <v>0.52</v>
@@ -1433,31 +1433,31 @@
         <v/>
       </c>
       <c r="E2" s="15" t="n">
-        <v>-0.01141700000000023</v>
+        <v>-0.01159600000000005</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>-0.002013993766835531</v>
+        <v>-0.002028522749806472</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>0.01896021861113817</v>
+        <v>0.01887370121015919</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.01509900546902498</v>
+        <v>0.01461270268334069</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.001857954662378591</v>
+        <v>-0.001953511908381</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>0.02787014483875128</v>
+        <v>0.02766701712668684</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>-0.006471060747739621</v>
+        <v>-0.006328720573457347</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.05710665510472102</v>
+        <v>0.05771769587240105</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.2101517284529959</v>
+        <v>0.2111248682033162</v>
       </c>
     </row>
     <row r="3">
@@ -1465,40 +1465,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.02370596042017659</v>
+        <v>-0.02566802823693404</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>0.1094568454500038</v>
+        <v>0.1097003085263357</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>0.132815340254709</v>
+        <v>0.1328115990357295</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>0.07498516318657411</v>
+        <v>0.07489560610399959</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>0.1208810867846097</v>
+        <v>0.1208179477933824</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>-0.04030668416552885</v>
+        <v>-0.04028579442287583</v>
       </c>
       <c r="H3" s="15" t="n">
-        <v>0.0008712609927179482</v>
+        <v>0.0008709267466799897</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.03972402158423005</v>
+        <v>0.04007758387696803</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>-0.03736194383086144</v>
+        <v>-0.03730785849091223</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>0.1829740526982524</v>
+        <v>0.1833285257979405</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>0.06611830284914322</v>
+        <v>0.06723082599993324</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.01773553899169034</v>
+        <v>-0.01774955492002017</v>
       </c>
     </row>
     <row r="4">
@@ -1506,40 +1506,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>-0.08277459440034762</v>
+        <v>-0.08277638778428942</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>0.0009017615059512263</v>
+        <v>0.000901508561540032</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>0.04671406954229629</v>
+        <v>0.04652437086018812</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>-0.02203992804956534</v>
+        <v>-0.02241877844702822</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>0.003916571219922726</v>
+        <v>0.003916338185182777</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>0.01195765759652545</v>
+        <v>0.01126967951664981</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.007607120840882553</v>
+        <v>0.007593462909938786</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.000182342502218491</v>
+        <v>-0.0002313717949341543</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>0.002577222377283528</v>
+        <v>0.002539015824873925</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>0.005819694369781248</v>
+        <v>0.005802881901583623</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>-0.001712616598299799</v>
+        <v>-0.001677915173877609</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>-0.005185453577319477</v>
+        <v>-0.005019701977257873</v>
       </c>
     </row>
     <row r="5">
@@ -1547,40 +1547,40 @@
         <v>2017</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>0.001301348315602802</v>
+        <v>0.001286978456636501</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>0.002788266535446393</v>
+        <v>0.002774829966924131</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.0006791319819534625</v>
+        <v>0.0008396416880991353</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.002287813863321997</v>
+        <v>0.002329253535584774</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>-0.001260089182988144</v>
+        <v>-0.001183494478786962</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>0.003671820725279717</v>
+        <v>0.003686933338975296</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.000220776131247824</v>
+        <v>0.0002296966598678285</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>0.00277423185328951</v>
+        <v>0.002775485973498748</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>0.002198104195302308</v>
+        <v>0.002294023890425656</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>0.002348293186456907</v>
+        <v>0.00233508184145137</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>-0.004032581270212887</v>
+        <v>-0.004449637892138036</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>-0.002226309378273617</v>
+        <v>-0.002225787880313801</v>
       </c>
     </row>
     <row r="6">
@@ -1588,40 +1588,40 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.02645794656771394</v>
+        <v>0.02669312797300272</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.02190034767405113</v>
+        <v>-0.02209594826414585</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>0.04390773180571728</v>
+        <v>0.0441638434671332</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>-0.02099428611103771</v>
+        <v>-0.02097697216561412</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>-0.01381156577647136</v>
+        <v>-0.01401210711720657</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>0.006034261295774446</v>
+        <v>0.006058940036699489</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>-0.01832534681911679</v>
+        <v>-0.01835653561279027</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>-0.03567806528250284</v>
+        <v>-0.03569263190244654</v>
       </c>
       <c r="J6" s="15" t="n">
-        <v>0.01919115048192777</v>
+        <v>0.01934414392101402</v>
       </c>
       <c r="K6" s="15" t="n">
-        <v>-0.03839198124028731</v>
+        <v>-0.03907205052447249</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>0.007501414463592315</v>
+        <v>0.007628858120808601</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.003577665893179649</v>
+        <v>0.003550062758061134</v>
       </c>
     </row>
     <row r="7">
@@ -1629,40 +1629,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>0.009071107734609951</v>
+        <v>0.008954997483388238</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>0.06653122350123919</v>
+        <v>0.06656865724202921</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0.06738165535350027</v>
+        <v>0.06731828458443645</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.01593085148894735</v>
+        <v>0.01565423337838268</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>-0.02658019923644117</v>
+        <v>-0.02680008589897376</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>0.0199468144214463</v>
+        <v>0.02035103346357037</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>0.005004567975677388</v>
+        <v>0.005111276712085555</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>0.0003595185290015124</v>
+        <v>0.0003497835566197427</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>0.0103868242830536</v>
+        <v>0.01048904822286456</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>0.003785497325269116</v>
+        <v>0.003799318794012851</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>0.007269295357427152</v>
+        <v>0.007257059505786589</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>0.01256475149966563</v>
+        <v>0.01251487635963455</v>
       </c>
     </row>
     <row r="8">
@@ -1670,40 +1670,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>0.01879249549711481</v>
+        <v>0.018899085088802</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>0.07842123251046829</v>
+        <v>0.07842736402178097</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-0.01529557353113065</v>
+        <v>-0.01525949756252887</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>0.03045222336935782</v>
+        <v>0.03041581108829572</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>0.00955779888368169</v>
+        <v>0.009668591465826104</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>0.05597459497369384</v>
+        <v>0.05578327057661792</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>0.08479985229566767</v>
+        <v>0.08497316091350737</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>-0.003074491032118876</v>
+        <v>-0.003206370375716694</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>-0.01361986665263759</v>
+        <v>-0.01363306649317886</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.03438971160263271</v>
+        <v>-0.03451161379971057</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.03118192771984196</v>
+        <v>0.03111934849201181</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>0.02895193558618292</v>
+        <v>0.02894426559702801</v>
       </c>
     </row>
     <row r="9">
@@ -1711,40 +1711,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>0.01103372587756457</v>
+        <v>0.01097202533036201</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>-0.03077460404762289</v>
+        <v>-0.03079863530415361</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.0005525010699842792</v>
+        <v>0.0005525163326587368</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>0.04582418989319836</v>
+        <v>0.04565195831239688</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>0.03850029474799466</v>
+        <v>0.03870620375522815</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>0.02475975071141101</v>
+        <v>0.02479687210770543</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>-0.04680934552813898</v>
+        <v>-0.04674654492007702</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>-0.02496118758927668</v>
+        <v>-0.02496155926086463</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.0167627717595622</v>
+        <v>-0.01681141992578705</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>0.007762229658705433</v>
+        <v>0.00773317198501422</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>0.01437757956786712</v>
+        <v>0.01447919279223697</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>-0.002559764767486206</v>
+        <v>-0.002906488410496788</v>
       </c>
     </row>
     <row r="10">
@@ -1752,25 +1752,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>-0.00133638589678764</v>
+        <v>-0.001333362616836031</v>
       </c>
       <c r="C10" s="15" t="n">
-        <v>0.0009736639920514545</v>
+        <v>0.0009734331459192447</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.0004250406356745007</v>
+        <v>0.0004252460269413838</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>0.001098059892287173</v>
+        <v>0.001100372907362646</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>0.03107843625921292</v>
+        <v>0.03112987822319968</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>0.1016176549075514</v>
+        <v>0.1016725634262066</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>-0.004704544843466718</v>
+        <v>-0.004741194651971092</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>
@@ -1889,31 +1889,31 @@
         <v/>
       </c>
       <c r="E2" s="15" t="n">
-        <v>0.05338055551199261</v>
+        <v>0.05319287953497609</v>
       </c>
       <c r="F2" s="15" t="n">
-        <v>-0.03271785268338745</v>
+        <v>-0.03273200118498287</v>
       </c>
       <c r="G2" s="15" t="n">
-        <v>-0.04682821799507264</v>
+        <v>-0.04691521325798353</v>
       </c>
       <c r="H2" s="15" t="n">
-        <v>0.0567677925978296</v>
+        <v>0.05627155309091236</v>
       </c>
       <c r="I2" s="15" t="n">
-        <v>-0.06051839991426877</v>
+        <v>-0.06061162267946607</v>
       </c>
       <c r="J2" s="15" t="n">
-        <v>-0.05165966984902171</v>
+        <v>-0.05184942700495221</v>
       </c>
       <c r="K2" s="15" t="n">
-        <v>0.01023193158243041</v>
+        <v>0.01038070130399293</v>
       </c>
       <c r="L2" s="15" t="n">
-        <v>0.01471046898503259</v>
+        <v>0.01529443939513087</v>
       </c>
       <c r="M2" s="15" t="n">
-        <v>0.2790255396981733</v>
+        <v>0.2800570027816152</v>
       </c>
     </row>
     <row r="3">
@@ -1921,40 +1921,40 @@
         <v>2015</v>
       </c>
       <c r="B3" s="15" t="n">
-        <v>-0.1508771868823964</v>
+        <v>-0.152582910102217</v>
       </c>
       <c r="C3" s="15" t="n">
-        <v>-0.03427201527301771</v>
+        <v>-0.03404231070888342</v>
       </c>
       <c r="D3" s="15" t="n">
-        <v>-0.06835506338022035</v>
+        <v>-0.06832532200595587</v>
       </c>
       <c r="E3" s="15" t="n">
-        <v>-0.129926375686357</v>
+        <v>-0.1299911755004153</v>
       </c>
       <c r="F3" s="15" t="n">
-        <v>-0.10267347395196</v>
+        <v>-0.1027294203452288</v>
       </c>
       <c r="G3" s="15" t="n">
-        <v>0.155521932430597</v>
+        <v>0.1555394587713028</v>
       </c>
       <c r="H3" s="15" t="n">
-        <v>0.08903084449131771</v>
+        <v>0.08903051040310705</v>
       </c>
       <c r="I3" s="15" t="n">
-        <v>0.2719380455567209</v>
+        <v>0.2723972010147266</v>
       </c>
       <c r="J3" s="15" t="n">
-        <v>-0.1039653710546969</v>
+        <v>-0.1039156176235343</v>
       </c>
       <c r="K3" s="15" t="n">
-        <v>-0.007413309815130886</v>
+        <v>-0.007052719898235194</v>
       </c>
       <c r="L3" s="15" t="n">
-        <v>-0.01610176637925076</v>
+        <v>-0.01507362932290257</v>
       </c>
       <c r="M3" s="15" t="n">
-        <v>-0.03472822458240232</v>
+        <v>-0.03474174706222621</v>
       </c>
     </row>
     <row r="4">
@@ -1962,40 +1962,40 @@
         <v>2016</v>
       </c>
       <c r="B4" s="15" t="n">
-        <v>0.2063566662881715</v>
+        <v>0.20635446050587</v>
       </c>
       <c r="C4" s="15" t="n">
-        <v>0.04636923549480998</v>
+        <v>0.04636904895949345</v>
       </c>
       <c r="D4" s="15" t="n">
-        <v>-0.1340117808769227</v>
+        <v>-0.1341721077992652</v>
       </c>
       <c r="E4" s="15" t="n">
-        <v>0.02013229197335176</v>
+        <v>0.01975716966162477</v>
       </c>
       <c r="F4" s="15" t="n">
-        <v>-0.01486098995672513</v>
+        <v>-0.01486122071320239</v>
       </c>
       <c r="G4" s="15" t="n">
-        <v>-0.02388861621350624</v>
+        <v>-0.02452141877972858</v>
       </c>
       <c r="H4" s="15" t="n">
-        <v>0.05321043396456493</v>
+        <v>0.053196165578411</v>
       </c>
       <c r="I4" s="15" t="n">
-        <v>-0.03420278435733703</v>
+        <v>-0.03425031301249204</v>
       </c>
       <c r="J4" s="15" t="n">
-        <v>0.02038537381838457</v>
+        <v>0.02034885630131988</v>
       </c>
       <c r="K4" s="15" t="n">
-        <v>-0.0001571923744969617</v>
+        <v>-0.0001739348090311621</v>
       </c>
       <c r="L4" s="15" t="n">
-        <v>-0.01366869426626272</v>
+        <v>-0.01363557077806865</v>
       </c>
       <c r="M4" s="15" t="n">
-        <v>0.1023003788845476</v>
+        <v>0.1024835895727314</v>
       </c>
     </row>
     <row r="5">
@@ -2003,40 +2003,40 @@
         <v>2017</v>
       </c>
       <c r="B5" s="15" t="n">
-        <v>0.03819804352718514</v>
+        <v>0.03818284919529646</v>
       </c>
       <c r="C5" s="15" t="n">
-        <v>-0.01930052556966488</v>
+        <v>-0.01931310160722821</v>
       </c>
       <c r="D5" s="15" t="n">
-        <v>0.009659138407765111</v>
+        <v>0.00981983507129347</v>
       </c>
       <c r="E5" s="15" t="n">
-        <v>0.03122372722630051</v>
+        <v>0.03126576045607332</v>
       </c>
       <c r="F5" s="15" t="n">
-        <v>0.04613083874717727</v>
+        <v>0.04621075307414091</v>
       </c>
       <c r="G5" s="15" t="n">
-        <v>-0.02808295615753809</v>
+        <v>-0.02806828295867303</v>
       </c>
       <c r="H5" s="15" t="n">
-        <v>0.04207685810447859</v>
+        <v>0.04208609454874201</v>
       </c>
       <c r="I5" s="15" t="n">
-        <v>-0.06052575973240337</v>
+        <v>-0.06052458765105218</v>
       </c>
       <c r="J5" s="15" t="n">
-        <v>-0.008180645752102422</v>
+        <v>-0.008085620611582467</v>
       </c>
       <c r="K5" s="15" t="n">
-        <v>-0.001105018089389009</v>
+        <v>-0.001119565862247818</v>
       </c>
       <c r="L5" s="15" t="n">
-        <v>0.04869107910846848</v>
+        <v>0.04825252855960716</v>
       </c>
       <c r="M5" s="15" t="n">
-        <v>0.005666512144770097</v>
+        <v>0.005667087269417559</v>
       </c>
     </row>
     <row r="6">
@@ -2044,40 +2044,40 @@
         <v>2018</v>
       </c>
       <c r="B6" s="15" t="n">
-        <v>0.03316993534385615</v>
+        <v>0.03340834904014578</v>
       </c>
       <c r="C6" s="15" t="n">
-        <v>-0.03955033723297097</v>
+        <v>-0.03973216226832543</v>
       </c>
       <c r="D6" s="15" t="n">
-        <v>-0.04040115275644429</v>
+        <v>-0.04018288206290088</v>
       </c>
       <c r="E6" s="15" t="n">
-        <v>0.02667007093878815</v>
+        <v>0.02668820762511204</v>
       </c>
       <c r="F6" s="15" t="n">
-        <v>0.01881603826145062</v>
+        <v>0.01860460801873876</v>
       </c>
       <c r="G6" s="15" t="n">
-        <v>0.08226442649476651</v>
+        <v>0.08229313751520384</v>
       </c>
       <c r="H6" s="15" t="n">
-        <v>0.006174338254247624</v>
+        <v>0.006141872906864076</v>
       </c>
       <c r="I6" s="15" t="n">
-        <v>0.04182697710174388</v>
+        <v>0.041811440659975</v>
       </c>
       <c r="J6" s="15" t="n">
-        <v>0.03447038936774161</v>
+        <v>0.03462313277916884</v>
       </c>
       <c r="K6" s="15" t="n">
-        <v>0.05340753623337369</v>
+        <v>0.05269482636938427</v>
       </c>
       <c r="L6" s="15" t="n">
-        <v>-0.03680619829029441</v>
+        <v>-0.03668326555471124</v>
       </c>
       <c r="M6" s="15" t="n">
-        <v>0.06408467673548923</v>
+        <v>0.06405612863754162</v>
       </c>
     </row>
     <row r="7">
@@ -2085,40 +2085,40 @@
         <v>2019</v>
       </c>
       <c r="B7" s="15" t="n">
-        <v>0.02461550557577774</v>
+        <v>0.02449736182949169</v>
       </c>
       <c r="C7" s="15" t="n">
-        <v>-0.1521788626271546</v>
+        <v>-0.1521481072372954</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>-0.03556270697348474</v>
+        <v>-0.03561913446202991</v>
       </c>
       <c r="E7" s="15" t="n">
-        <v>0.05664057526112565</v>
+        <v>0.05636210503886563</v>
       </c>
       <c r="F7" s="15" t="n">
-        <v>0.05416183015333287</v>
+        <v>0.05394177729962424</v>
       </c>
       <c r="G7" s="15" t="n">
-        <v>-0.002355094581348971</v>
+        <v>-0.001950740386560068</v>
       </c>
       <c r="H7" s="15" t="n">
-        <v>-0.03534396423137098</v>
+        <v>-0.03524071083529701</v>
       </c>
       <c r="I7" s="15" t="n">
-        <v>-0.02743763303429414</v>
+        <v>-0.02744706163861788</v>
       </c>
       <c r="J7" s="15" t="n">
-        <v>-0.002716761536478374</v>
+        <v>-0.002613636941407704</v>
       </c>
       <c r="K7" s="15" t="n">
-        <v>-0.02442296479214556</v>
+        <v>-0.02440960607726828</v>
       </c>
       <c r="L7" s="15" t="n">
-        <v>0.009108577891234759</v>
+        <v>0.00909704505221276</v>
       </c>
       <c r="M7" s="15" t="n">
-        <v>-0.0647068579620631</v>
+        <v>-0.06475112975489938</v>
       </c>
     </row>
     <row r="8">
@@ -2126,40 +2126,40 @@
         <v>2020</v>
       </c>
       <c r="B8" s="15" t="n">
-        <v>-0.05273264730386928</v>
+        <v>-0.05263164150865873</v>
       </c>
       <c r="C8" s="15" t="n">
-        <v>-0.003048353300620588</v>
+        <v>-0.003042201221338692</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>0.07949663184902933</v>
+        <v>0.07953705635684005</v>
       </c>
       <c r="E8" s="15" t="n">
-        <v>-0.07196587685914502</v>
+        <v>-0.07199823661419424</v>
       </c>
       <c r="F8" s="15" t="n">
-        <v>-0.001063467657272277</v>
+        <v>-0.0009507954286902542</v>
       </c>
       <c r="G8" s="15" t="n">
-        <v>-0.09843364153000167</v>
+        <v>-0.09860324922752561</v>
       </c>
       <c r="H8" s="15" t="n">
-        <v>-0.05978796462066494</v>
+        <v>-0.05963247172181108</v>
       </c>
       <c r="I8" s="15" t="n">
-        <v>0.01786792531143999</v>
+        <v>0.0177386681859979</v>
       </c>
       <c r="J8" s="15" t="n">
-        <v>0.03936970938950579</v>
+        <v>0.03935641307055393</v>
       </c>
       <c r="K8" s="15" t="n">
-        <v>-0.06773090424224038</v>
+        <v>-0.06784504574716388</v>
       </c>
       <c r="L8" s="15" t="n">
-        <v>0.03701782087645489</v>
+        <v>0.03695710742738334</v>
       </c>
       <c r="M8" s="15" t="n">
-        <v>-0.09042684179818528</v>
+        <v>-0.09043479030454038</v>
       </c>
     </row>
     <row r="9">
@@ -2167,40 +2167,40 @@
         <v>2021</v>
       </c>
       <c r="B9" s="15" t="n">
-        <v>-0.04574870540786391</v>
+        <v>-0.04580452078665742</v>
       </c>
       <c r="C9" s="15" t="n">
-        <v>0.03822039121878351</v>
+        <v>0.03819522515999862</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0.04348864596969193</v>
+        <v>0.04348865328704266</v>
       </c>
       <c r="E9" s="15" t="n">
-        <v>-0.06891203217601727</v>
+        <v>-0.06906215675298</v>
       </c>
       <c r="F9" s="15" t="n">
-        <v>-0.03248379934036894</v>
+        <v>-0.03228752057337403</v>
       </c>
       <c r="G9" s="15" t="n">
-        <v>-0.02729478458425716</v>
+        <v>-0.0272598178967276</v>
       </c>
       <c r="H9" s="15" t="n">
-        <v>-0.04330865855918242</v>
+        <v>-0.04324606353327654</v>
       </c>
       <c r="I9" s="15" t="n">
-        <v>0.03933761512023448</v>
+        <v>0.03933726870946774</v>
       </c>
       <c r="J9" s="15" t="n">
-        <v>-0.03026001456668015</v>
+        <v>-0.03030753639618611</v>
       </c>
       <c r="K9" s="15" t="n">
-        <v>-0.02601632742015592</v>
+        <v>-0.02604381864871042</v>
       </c>
       <c r="L9" s="15" t="n">
-        <v>-0.02879163471071344</v>
+        <v>-0.02869322671457242</v>
       </c>
       <c r="M9" s="15" t="n">
-        <v>0.04628910432036992</v>
+        <v>0.0459328390578333</v>
       </c>
     </row>
     <row r="10">
@@ -2208,25 +2208,25 @@
         <v>2022</v>
       </c>
       <c r="B10" s="15" t="n">
-        <v>0.134447811629697</v>
+        <v>0.1344511766287664</v>
       </c>
       <c r="C10" s="15" t="n">
-        <v>0.00526438313152533</v>
+        <v>0.005264139874611162</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0.07054428171048399</v>
+        <v>0.07054447303678923</v>
       </c>
       <c r="E10" s="15" t="n">
-        <v>0.1326699334146857</v>
+        <v>0.1326725459947038</v>
       </c>
       <c r="F10" s="15" t="n">
-        <v>-0.01004467772400208</v>
+        <v>-0.00999414125095377</v>
       </c>
       <c r="G10" s="15" t="n">
-        <v>-0.05971541996102403</v>
+        <v>-0.05966201534272408</v>
       </c>
       <c r="H10" s="15" t="n">
-        <v>0.005491886090827069</v>
+        <v>0.005455236282322584</v>
       </c>
       <c r="I10" s="15" t="n">
         <v/>

</xml_diff>